<commit_message>
added more info in vugen
</commit_message>
<xml_diff>
--- a/Chandrakala_Required.xlsx
+++ b/Chandrakala_Required.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="570">
   <si>
     <t>Sl No</t>
   </si>
@@ -2115,6 +2115,18 @@
   </si>
   <si>
     <t>difference between wiinet and socket</t>
+  </si>
+  <si>
+    <t>Git Integration</t>
+  </si>
+  <si>
+    <t>little's law:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pacing </t>
+  </si>
+  <si>
+    <t>N= Z*(R+T)</t>
   </si>
 </sst>
 </file>
@@ -3240,6 +3252,44 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>151924</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>152071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="11811000"/>
+          <a:ext cx="3809524" cy="2628571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4291,10 +4341,10 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A2:G31"/>
+  <dimension ref="A2:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4422,6 +4472,26 @@
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>565</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>